<commit_message>
add image, FFAffiliation, change name btn all, process iamge in model
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WindownFormApplication\WFA_PrincessConnectReDive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E9BC380-373C-4589-9A11-7B27194F3B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13B9162-B517-48AA-A9E5-8D1B87C736BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="4170" windowWidth="21600" windowHeight="11385" xr2:uid="{935D6C5E-0CFC-4A6C-B32D-E4FF1E41311B}"/>
+    <workbookView xWindow="3600" yWindow="3990" windowWidth="21600" windowHeight="11385" xr2:uid="{935D6C5E-0CFC-4A6C-B32D-E4FF1E41311B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="184">
   <si>
     <t>chara_01_01</t>
   </si>
@@ -512,6 +512,72 @@
   </si>
   <si>
     <t>"}</t>
+  </si>
+  <si>
+    <t>Guild</t>
+  </si>
+  <si>
+    <t>","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"</t>
+  </si>
+  <si>
+    <t>chara_16_02</t>
+  </si>
+  <si>
+    <t>คาริน</t>
+  </si>
+  <si>
+    <t>chara_16_03</t>
+  </si>
+  <si>
+    <t>มุอิมิ</t>
+  </si>
+  <si>
+    <t>chara_16_04</t>
+  </si>
+  <si>
+    <t>อาเมส</t>
+  </si>
+  <si>
+    <t>chara_18_01</t>
+  </si>
+  <si>
+    <t>ไคเซอร์อินไซท์</t>
+  </si>
+  <si>
+    <t>chara_16_01</t>
+  </si>
+  <si>
+    <t>อ็อคโต้</t>
+  </si>
+  <si>
+    <t>btn_16_01</t>
+  </si>
+  <si>
+    <t>btn_16_02</t>
+  </si>
+  <si>
+    <t>btn_16_03</t>
+  </si>
+  <si>
+    <t>btn_16_04</t>
+  </si>
+  <si>
+    <t>btn_18_01</t>
+  </si>
+  <si>
+    <t>", "UnionBurst": "</t>
+  </si>
+  <si>
+    <t>","Skill1": "</t>
+  </si>
+  <si>
+    <t>","Skill2": "</t>
+  </si>
+  <si>
+    <t>","EXSkill": "</t>
+  </si>
+  <si>
+    <t>FFAffiliation</t>
   </si>
 </sst>
 </file>
@@ -2316,10 +2382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DEEA7C-D346-48E9-BEA1-5F2F7E5F06C5}">
-  <dimension ref="D2:T64"/>
+  <dimension ref="D2:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20:T64"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,7 +2395,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -2342,7 +2408,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
     </row>
-    <row r="3" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2355,7 +2421,7 @@
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
     </row>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2440,7 @@
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2393,7 +2459,7 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2412,7 +2478,7 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2434,8 +2500,10 @@
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
-    </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2457,8 +2525,10 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+    </row>
+    <row r="9" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2480,8 +2550,10 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
-    </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
@@ -2503,8 +2575,10 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
-    </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+    </row>
+    <row r="11" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2526,8 +2600,10 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
-    </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+    </row>
+    <row r="12" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D12" s="8" t="s">
         <v>16</v>
       </c>
@@ -2549,8 +2625,10 @@
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
-    </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+    </row>
+    <row r="13" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2568,7 +2646,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2586,7 +2664,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
@@ -2604,7 +2682,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
@@ -2622,7 +2700,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2640,7 +2718,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
@@ -2658,7 +2736,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
@@ -2677,11 +2755,13 @@
       <c r="R19" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="T19" t="s">
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="V19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>32</v>
       </c>
@@ -2725,14 +2805,20 @@
         <v>3</v>
       </c>
       <c r="S20" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U20" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T20" t="str">
-        <f>CONCATENATE(G20,H20,I20,J20,K20,L20,M20,N20,O20,P20,Q20,R20,S20)</f>
-        <v xml:space="preserve"> {"Charc": "chara_01_01","BtnCharac": "btn_01_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_01","EXSkill": "EXSkill_03"},</v>
-      </c>
-    </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="V20" t="str">
+        <f>CONCATENATE(G20,H20,I20,J20,K20,L20,M20,N20,O20,P20,Q20,R20,S20,T20,U20)</f>
+        <v xml:space="preserve"> {"Charc": "chara_01_01","BtnCharac": "btn_01_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_01","EXSkill": "EXSkill_03","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
         <v>34</v>
       </c>
@@ -2776,14 +2862,20 @@
         <v>5</v>
       </c>
       <c r="S21" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U21" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T21" t="str">
-        <f t="shared" ref="T21:T64" si="0">CONCATENATE(G21,H21,I21,J21,K21,L21,M21,N21,O21,P21,Q21,R21,S21)</f>
-        <v xml:space="preserve"> {"Charc": "chara_01_02","BtnCharac": "btn_01_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_06","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="22" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="V21" t="str">
+        <f t="shared" ref="V21:V64" si="0">CONCATENATE(G21,H21,I21,J21,K21,L21,M21,N21,O21,P21,Q21,R21,S21,T21,U21)</f>
+        <v xml:space="preserve"> {"Charc": "chara_01_02","BtnCharac": "btn_01_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_06","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
@@ -2827,14 +2919,20 @@
         <v>1</v>
       </c>
       <c r="S22" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U22" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T22" t="str">
+      <c r="V22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_01_03","BtnCharac": "btn_01_03", "UnionBurst": "UnionBurst_02","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_01_03","BtnCharac": "btn_01_03", "UnionBurst": "UnionBurst_02","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -2878,14 +2976,20 @@
         <v>1</v>
       </c>
       <c r="S23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U23" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T23" t="str">
+      <c r="V23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_02_01","BtnCharac": "btn_02_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="24" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_02_01","BtnCharac": "btn_02_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>40</v>
       </c>
@@ -2929,14 +3033,20 @@
         <v>5</v>
       </c>
       <c r="S24" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T24" t="str">
+      <c r="V24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_02_02","BtnCharac": "btn_02_02", "UnionBurst": "UnionBurst_02","Skill1": "Skill_12","Skill2": "Skill_03","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="25" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_02_02","BtnCharac": "btn_02_02", "UnionBurst": "UnionBurst_02","Skill1": "Skill_12","Skill2": "Skill_03","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>42</v>
       </c>
@@ -2980,14 +3090,20 @@
         <v>1</v>
       </c>
       <c r="S25" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U25" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T25" t="str">
+      <c r="V25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_02_03","BtnCharac": "btn_02_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="26" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_02_03","BtnCharac": "btn_02_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D26" s="2" t="s">
         <v>44</v>
       </c>
@@ -3031,14 +3147,20 @@
         <v>4</v>
       </c>
       <c r="S26" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U26" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T26" t="str">
+      <c r="V26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_03_02","BtnCharac": "btn_03_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_04","Skill2": "Skill_16","EXSkill": "EXSkill_04"},</v>
-      </c>
-    </row>
-    <row r="27" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_03_02","BtnCharac": "btn_03_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_04","Skill2": "Skill_16","EXSkill": "EXSkill_04","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
@@ -3082,14 +3204,20 @@
         <v>1</v>
       </c>
       <c r="S27" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U27" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T27" t="str">
+      <c r="V27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_03_03","BtnCharac": "btn_03_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="28" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_03_03","BtnCharac": "btn_03_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
         <v>48</v>
       </c>
@@ -3132,15 +3260,21 @@
       <c r="R28" s="9">
         <v>4</v>
       </c>
-      <c r="S28" s="10" t="s">
+      <c r="S28" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U28" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T28" t="str">
+      <c r="V28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_04_01","BtnCharac": "btn_04_01", "UnionBurst": "UnionBurst_03","Skill1": "Skill_07","Skill2": "Skill_04","EXSkill": "EXSkill_04"},</v>
-      </c>
-    </row>
-    <row r="29" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_04_01","BtnCharac": "btn_04_01", "UnionBurst": "UnionBurst_03","Skill1": "Skill_07","Skill2": "Skill_04","EXSkill": "EXSkill_04","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D29" s="2" t="s">
         <v>50</v>
       </c>
@@ -3184,14 +3318,20 @@
         <v>5</v>
       </c>
       <c r="S29" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U29" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T29" t="str">
+      <c r="V29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_04_02","BtnCharac": "btn_04_02", "UnionBurst": "UnionBurst_02","Skill1": "Skill_03","Skill2": "Skill_06","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="30" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_04_02","BtnCharac": "btn_04_02", "UnionBurst": "UnionBurst_02","Skill1": "Skill_03","Skill2": "Skill_06","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
         <v>52</v>
       </c>
@@ -3235,14 +3375,20 @@
         <v>1</v>
       </c>
       <c r="S30" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U30" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T30" t="str">
+      <c r="V30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_05_01","BtnCharac": "btn_05_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="31" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_05_01","BtnCharac": "btn_05_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D31" s="2" t="s">
         <v>54</v>
       </c>
@@ -3286,14 +3432,20 @@
         <v>4</v>
       </c>
       <c r="S31" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U31" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T31" t="str">
+      <c r="V31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_05_03","BtnCharac": "btn_05_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_11","Skill2": "Skill_06","EXSkill": "EXSkill_04"},</v>
-      </c>
-    </row>
-    <row r="32" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_05_03","BtnCharac": "btn_05_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_11","Skill2": "Skill_06","EXSkill": "EXSkill_04","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D32" s="2" t="s">
         <v>56</v>
       </c>
@@ -3337,14 +3489,20 @@
         <v>1</v>
       </c>
       <c r="S32" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U32" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T32" t="str">
+      <c r="V32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_06_01","BtnCharac": "btn_06_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_10","Skill2": "Skill_14","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_06_01","BtnCharac": "btn_06_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_10","Skill2": "Skill_14","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
         <v>58</v>
       </c>
@@ -3388,14 +3546,20 @@
         <v>5</v>
       </c>
       <c r="S33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U33" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T33" t="str">
+      <c r="V33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_06_03","BtnCharac": "btn_06_03", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_12","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_06_03","BtnCharac": "btn_06_03", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_12","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
         <v>60</v>
       </c>
@@ -3439,14 +3603,20 @@
         <v>5</v>
       </c>
       <c r="S34" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U34" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T34" t="str">
+      <c r="V34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_07_02","BtnCharac": "btn_07_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_03","Skill2": "Skill_12","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_07_02","BtnCharac": "btn_07_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_03","Skill2": "Skill_12","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
         <v>62</v>
       </c>
@@ -3490,14 +3660,20 @@
         <v>5</v>
       </c>
       <c r="S35" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U35" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T35" t="str">
+      <c r="V35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_07_03","BtnCharac": "btn_07_03", "UnionBurst": "UnionBurst_03","Skill1": "Skill_12","Skill2": "Skill_06","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="36" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_07_03","BtnCharac": "btn_07_03", "UnionBurst": "UnionBurst_03","Skill1": "Skill_12","Skill2": "Skill_06","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
         <v>64</v>
       </c>
@@ -3541,14 +3717,20 @@
         <v>1</v>
       </c>
       <c r="S36" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T36" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U36" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T36" t="str">
+      <c r="V36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_07_04","BtnCharac": "btn_07_04", "UnionBurst": "UnionBurst_01","Skill1": "Skill_05","Skill2": "Skill_06","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="37" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_07_04","BtnCharac": "btn_07_04", "UnionBurst": "UnionBurst_01","Skill1": "Skill_05","Skill2": "Skill_06","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D37" s="2" t="s">
         <v>66</v>
       </c>
@@ -3592,14 +3774,20 @@
         <v>4</v>
       </c>
       <c r="S37" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U37" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T37" t="str">
+      <c r="V37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_07_05","BtnCharac": "btn_07_05", "UnionBurst": "UnionBurst_01","Skill1": "Skill_05","Skill2": "Skill_04","EXSkill": "EXSkill_04"},</v>
-      </c>
-    </row>
-    <row r="38" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_07_05","BtnCharac": "btn_07_05", "UnionBurst": "UnionBurst_01","Skill1": "Skill_05","Skill2": "Skill_04","EXSkill": "EXSkill_04","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
         <v>68</v>
       </c>
@@ -3643,14 +3831,20 @@
         <v>2</v>
       </c>
       <c r="S38" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U38" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T38" t="str">
+      <c r="V38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_08_01","BtnCharac": "btn_08_01", "UnionBurst": "UnionBurst_04","Skill1": "Skill_04","Skill2": "Skill_01","EXSkill": "EXSkill_02"},</v>
-      </c>
-    </row>
-    <row r="39" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_08_01","BtnCharac": "btn_08_01", "UnionBurst": "UnionBurst_04","Skill1": "Skill_04","Skill2": "Skill_01","EXSkill": "EXSkill_02","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D39" s="2" t="s">
         <v>70</v>
       </c>
@@ -3694,14 +3888,20 @@
         <v>1</v>
       </c>
       <c r="S39" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T39" t="str">
+      <c r="V39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_09_01","BtnCharac": "btn_09_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="40" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_09_01","BtnCharac": "btn_09_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="40" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
         <v>72</v>
       </c>
@@ -3745,14 +3945,20 @@
         <v>5</v>
       </c>
       <c r="S40" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T40" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U40" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T40" t="str">
+      <c r="V40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_09_02","BtnCharac": "btn_09_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_04","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="41" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_09_02","BtnCharac": "btn_09_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_04","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
         <v>74</v>
       </c>
@@ -3796,14 +4002,20 @@
         <v>3</v>
       </c>
       <c r="S41" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T41" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U41" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T41" t="str">
+      <c r="V41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_09_04","BtnCharac": "btn_09_04", "UnionBurst": "UnionBurst_05","Skill1": "Skill_03","Skill2": "Skill_07","EXSkill": "EXSkill_03"},</v>
-      </c>
-    </row>
-    <row r="42" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_09_04","BtnCharac": "btn_09_04", "UnionBurst": "UnionBurst_05","Skill1": "Skill_03","Skill2": "Skill_07","EXSkill": "EXSkill_03","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
         <v>76</v>
       </c>
@@ -3847,14 +4059,20 @@
         <v>4</v>
       </c>
       <c r="S42" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T42" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U42" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T42" t="str">
+      <c r="V42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_10_01","BtnCharac": "btn_10_01", "UnionBurst": "UnionBurst_03","Skill1": "Skill_04","Skill2": "Skill_11","EXSkill": "EXSkill_04"},</v>
-      </c>
-    </row>
-    <row r="43" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_10_01","BtnCharac": "btn_10_01", "UnionBurst": "UnionBurst_03","Skill1": "Skill_04","Skill2": "Skill_11","EXSkill": "EXSkill_04","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">
         <v>78</v>
       </c>
@@ -3898,14 +4116,20 @@
         <v>1</v>
       </c>
       <c r="S43" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U43" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T43" t="str">
+      <c r="V43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_10_02","BtnCharac": "btn_10_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_06","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="44" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_10_02","BtnCharac": "btn_10_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_06","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
         <v>80</v>
       </c>
@@ -3949,14 +4173,20 @@
         <v>1</v>
       </c>
       <c r="S44" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T44" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U44" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T44" t="str">
+      <c r="V44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_10_03","BtnCharac": "btn_10_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_10_03","BtnCharac": "btn_10_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="45" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D45" s="2" t="s">
         <v>82</v>
       </c>
@@ -4000,14 +4230,20 @@
         <v>1</v>
       </c>
       <c r="S45" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T45" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U45" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T45" t="str">
+      <c r="V45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_11_01","BtnCharac": "btn_11_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="46" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_11_01","BtnCharac": "btn_11_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="46" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
         <v>84</v>
       </c>
@@ -4051,14 +4287,20 @@
         <v>4</v>
       </c>
       <c r="S46" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T46" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U46" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T46" t="str">
+      <c r="V46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_11_02","BtnCharac": "btn_11_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_04"},</v>
-      </c>
-    </row>
-    <row r="47" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_11_02","BtnCharac": "btn_11_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_04","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="47" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D47" s="8" t="s">
         <v>86</v>
       </c>
@@ -4102,14 +4344,20 @@
         <v>1</v>
       </c>
       <c r="S47" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T47" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U47" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T47" t="str">
+      <c r="V47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_11_03","BtnCharac": "btn_11_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="48" spans="4:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_11_03","BtnCharac": "btn_11_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="48" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
         <v>88</v>
       </c>
@@ -4153,14 +4401,20 @@
         <v>2</v>
       </c>
       <c r="S48" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U48" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T48" t="str">
+      <c r="V48" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_11_04","BtnCharac": "btn_11_04", "UnionBurst": "UnionBurst_03","Skill1": "Skill_03","Skill2": "Skill_07","EXSkill": "EXSkill_02"},</v>
-      </c>
-    </row>
-    <row r="49" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_11_04","BtnCharac": "btn_11_04", "UnionBurst": "UnionBurst_03","Skill1": "Skill_03","Skill2": "Skill_07","EXSkill": "EXSkill_02","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="49" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>142</v>
       </c>
@@ -4198,14 +4452,20 @@
         <v>1</v>
       </c>
       <c r="S49" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T49" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U49" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T49" t="str">
+      <c r="V49" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_12_01","BtnCharac": "btn_12_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_15","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="50" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_12_01","BtnCharac": "btn_12_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_15","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="50" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>142</v>
       </c>
@@ -4243,14 +4503,20 @@
         <v>1</v>
       </c>
       <c r="S50" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U50" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T50" t="str">
+      <c r="V50" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_12_02","BtnCharac": "btn_12_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_04","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="51" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_12_02","BtnCharac": "btn_12_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_04","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="51" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>142</v>
       </c>
@@ -4288,14 +4554,20 @@
         <v>2</v>
       </c>
       <c r="S51" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T51" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U51" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T51" t="str">
+      <c r="V51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_12_03","BtnCharac": "btn_12_03", "UnionBurst": "UnionBurst_04","Skill1": "Skill_04","Skill2": "Skill_02","EXSkill": "EXSkill_02"},</v>
-      </c>
-    </row>
-    <row r="52" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_12_03","BtnCharac": "btn_12_03", "UnionBurst": "UnionBurst_04","Skill1": "Skill_04","Skill2": "Skill_02","EXSkill": "EXSkill_02","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="52" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>142</v>
       </c>
@@ -4333,14 +4605,20 @@
         <v>1</v>
       </c>
       <c r="S52" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T52" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U52" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T52" t="str">
+      <c r="V52" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_12_04","BtnCharac": "btn_12_04", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="53" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_12_04","BtnCharac": "btn_12_04", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="53" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>142</v>
       </c>
@@ -4378,14 +4656,20 @@
         <v>1</v>
       </c>
       <c r="S53" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U53" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T53" t="str">
+      <c r="V53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_13_02","BtnCharac": "btn_13_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_08","Skill2": "Skill_09","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="54" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_13_02","BtnCharac": "btn_13_02", "UnionBurst": "UnionBurst_01","Skill1": "Skill_08","Skill2": "Skill_09","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="54" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>142</v>
       </c>
@@ -4423,14 +4707,20 @@
         <v>1</v>
       </c>
       <c r="S54" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U54" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T54" t="str">
+      <c r="V54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_13_03","BtnCharac": "btn_13_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_10","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="55" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_13_03","BtnCharac": "btn_13_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_10","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="55" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>142</v>
       </c>
@@ -4468,14 +4758,20 @@
         <v>5</v>
       </c>
       <c r="S55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T55" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U55" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T55" t="str">
+      <c r="V55" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_13_05","BtnCharac": "btn_13_05", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_05","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="56" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_13_05","BtnCharac": "btn_13_05", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_05","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="56" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>142</v>
       </c>
@@ -4513,14 +4809,20 @@
         <v>5</v>
       </c>
       <c r="S56" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T56" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U56" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T56" t="str">
+      <c r="V56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_14_01","BtnCharac": "btn_14_01", "UnionBurst": "UnionBurst_07","Skill1": "Skill_12","Skill2": "Skill_02","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="57" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_14_01","BtnCharac": "btn_14_01", "UnionBurst": "UnionBurst_07","Skill1": "Skill_12","Skill2": "Skill_02","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="57" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
         <v>142</v>
       </c>
@@ -4558,14 +4860,20 @@
         <v>5</v>
       </c>
       <c r="S57" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T57" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U57" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T57" t="str">
+      <c r="V57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_14_02","BtnCharac": "btn_14_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_12","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="58" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_14_02","BtnCharac": "btn_14_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_12","Skill2": "Skill_12","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="58" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
         <v>142</v>
       </c>
@@ -4603,14 +4911,20 @@
         <v>1</v>
       </c>
       <c r="S58" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T58" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U58" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T58" t="str">
+      <c r="V58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_14_03","BtnCharac": "btn_14_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="59" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_14_03","BtnCharac": "btn_14_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_03","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="59" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>142</v>
       </c>
@@ -4648,14 +4962,20 @@
         <v>1</v>
       </c>
       <c r="S59" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T59" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U59" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T59" t="str">
+      <c r="V59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_15_01","BtnCharac": "btn_15_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="60" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_15_01","BtnCharac": "btn_15_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_03","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="60" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
         <v>142</v>
       </c>
@@ -4693,14 +5013,20 @@
         <v>5</v>
       </c>
       <c r="S60" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T60" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U60" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T60" t="str">
+      <c r="V60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_15_02","BtnCharac": "btn_15_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_11","Skill2": "Skill_02","EXSkill": "EXSkill_05"},</v>
-      </c>
-    </row>
-    <row r="61" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_15_02","BtnCharac": "btn_15_02", "UnionBurst": "UnionBurst_06","Skill1": "Skill_11","Skill2": "Skill_02","EXSkill": "EXSkill_05","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="61" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
         <v>142</v>
       </c>
@@ -4738,14 +5064,20 @@
         <v>1</v>
       </c>
       <c r="S61" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T61" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U61" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T61" t="str">
+      <c r="V61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_15_03","BtnCharac": "btn_15_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="62" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_15_03","BtnCharac": "btn_15_03", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_01","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="62" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
         <v>142</v>
       </c>
@@ -4783,14 +5115,20 @@
         <v>2</v>
       </c>
       <c r="S62" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T62" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U62" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T62" t="str">
+      <c r="V62" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_15_04","BtnCharac": "btn_15_04", "UnionBurst": "UnionBurst_04","Skill1": "Skill_13","Skill2": "Skill_03","EXSkill": "EXSkill_02"},</v>
-      </c>
-    </row>
-    <row r="63" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_15_04","BtnCharac": "btn_15_04", "UnionBurst": "UnionBurst_04","Skill1": "Skill_13","Skill2": "Skill_03","EXSkill": "EXSkill_02","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="63" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G63" s="9" t="s">
         <v>142</v>
       </c>
@@ -4827,15 +5165,21 @@
       <c r="R63" s="9">
         <v>1</v>
       </c>
-      <c r="S63" s="10" t="s">
+      <c r="S63" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T63" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U63" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T63" t="str">
+      <c r="V63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_17_01","BtnCharac": "btn_17_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01"},</v>
-      </c>
-    </row>
-    <row r="64" spans="7:20" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> {"Charc": "chara_17_01","BtnCharac": "btn_17_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"},</v>
+      </c>
+    </row>
+    <row r="64" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
         <v>142</v>
       </c>
@@ -4873,11 +5217,252 @@
         <v>1</v>
       </c>
       <c r="S64" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T64" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="U64" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="T64" t="str">
+      <c r="V64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> {"Charc": "chara_19_01","BtnCharac": "btn_19_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01"}</v>
+        <v xml:space="preserve"> {"Charc": "chara_19_01","BtnCharac": "btn_19_01", "UnionBurst": "UnionBurst_01","Skill1": "Skill_01","Skill2": "Skill_02","EXSkill": "EXSkill_01","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"Guild"}</v>
+      </c>
+    </row>
+    <row r="67" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>172</v>
+      </c>
+      <c r="E67" t="s">
+        <v>173</v>
+      </c>
+      <c r="G67" t="s">
+        <v>142</v>
+      </c>
+      <c r="H67" t="s">
+        <v>172</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M67" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="S67" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T67" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U67" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="V67" t="str">
+        <f t="shared" ref="V67:V71" si="1">CONCATENATE(G67,H67,I67,J67,K67,L67,M67,N67,O67,P67,Q67,R67,S67,T67,U67)</f>
+        <v xml:space="preserve"> {"Charc": "chara_16_01","BtnCharac": "btn_16_01", "UnionBurst": "","Skill1": "","Skill2": "","EXSkill": "","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"FFAffiliation"}</v>
+      </c>
+    </row>
+    <row r="68" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>164</v>
+      </c>
+      <c r="E68" t="s">
+        <v>165</v>
+      </c>
+      <c r="G68" t="s">
+        <v>142</v>
+      </c>
+      <c r="H68" t="s">
+        <v>164</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J68" t="s">
+        <v>175</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M68" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T68" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="V68" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> {"Charc": "chara_16_02","BtnCharac": "btn_16_02", "UnionBurst": "","Skill1": "","Skill2": "","EXSkill": "","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"FFAffiliation"}</v>
+      </c>
+    </row>
+    <row r="69" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>166</v>
+      </c>
+      <c r="E69" t="s">
+        <v>167</v>
+      </c>
+      <c r="G69" t="s">
+        <v>142</v>
+      </c>
+      <c r="H69" t="s">
+        <v>166</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J69" t="s">
+        <v>176</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M69" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="S69" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T69" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U69" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="V69" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> {"Charc": "chara_16_03","BtnCharac": "btn_16_03", "UnionBurst": "","Skill1": "","Skill2": "","EXSkill": "","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"FFAffiliation"}</v>
+      </c>
+    </row>
+    <row r="70" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>168</v>
+      </c>
+      <c r="E70" t="s">
+        <v>169</v>
+      </c>
+      <c r="G70" t="s">
+        <v>142</v>
+      </c>
+      <c r="H70" t="s">
+        <v>168</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J70" t="s">
+        <v>177</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M70" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T70" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U70" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="V70" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> {"Charc": "chara_16_04","BtnCharac": "btn_16_04", "UnionBurst": "","Skill1": "","Skill2": "","EXSkill": "","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"FFAffiliation"}</v>
+      </c>
+    </row>
+    <row r="71" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>170</v>
+      </c>
+      <c r="E71" t="s">
+        <v>171</v>
+      </c>
+      <c r="G71" t="s">
+        <v>142</v>
+      </c>
+      <c r="H71" t="s">
+        <v>170</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J71" t="s">
+        <v>178</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M71" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="S71" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="T71" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U71" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="V71" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> {"Charc": "chara_18_01","BtnCharac": "btn_18_01", "UnionBurst": "","Skill1": "","Skill2": "","EXSkill": "","GifUnionBurst": "","GifSkill1":"","GifSkill2":"","Type":"FFAffiliation"}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>